<commit_message>
updated with extra comments and renamed the main file
</commit_message>
<xml_diff>
--- a/input_excel_file.xlsx
+++ b/input_excel_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Data Analytics\QP_Format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCCE3EB-2C67-4DEA-AE09-6A82889492F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4902F7-B926-420E-B442-47295B6D68A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="86">
   <si>
     <t>Q_No</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>- PM</t>
+  </si>
+  <si>
+    <t>4A</t>
   </si>
 </sst>
 </file>
@@ -634,8 +637,8 @@
   </sheetPr>
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -865,7 +868,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="B11">
         <v>8</v>

</xml_diff>